<commit_message>
First Final Version of The Project
</commit_message>
<xml_diff>
--- a/data_in/insurance_taxonomy.xlsx
+++ b/data_in/insurance_taxonomy.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttioa\OneDrive\Documente\Proiect Veridion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttioa\OneDrive\Documente\Proiect Veridion\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDA74A1A-C3FD-4799-BBC8-9382D8B98619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55B411B-1353-4699-96A6-CC2856333F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FFD84A5A-B61A-493B-BCF3-7011055BFBFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$221</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1077,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95E255B-85B5-4550-BD46-B397CEE3167F}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="K214" sqref="K214"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,7 +1164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>174</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>215</v>
       </c>
@@ -4529,6 +4532,8 @@
       <c r="A1000" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A221" xr:uid="{E95E255B-85B5-4550-BD46-B397CEE3167F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>